<commit_message>
Update 2014 vaccination timing
</commit_message>
<xml_diff>
--- a/data/Bentiu population.xlsx
+++ b/data/Bentiu population.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22400" windowHeight="20460" tabRatio="500"/>
@@ -159,8 +159,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,13 +179,15 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,11 +422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="361685272"/>
-        <c:axId val="361688296"/>
+        <c:axId val="2103639656"/>
+        <c:axId val="2103642680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="361685272"/>
+        <c:axId val="2103639656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,12 +436,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361688296"/>
+        <c:crossAx val="2103642680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="361688296"/>
+        <c:axId val="2103642680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361685272"/>
+        <c:crossAx val="2103639656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -480,7 +484,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -702,11 +705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120468296"/>
-        <c:axId val="121877640"/>
+        <c:axId val="2103717592"/>
+        <c:axId val="2103720648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120468296"/>
+        <c:axId val="2103717592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,12 +719,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121877640"/>
+        <c:crossAx val="2103720648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121877640"/>
+        <c:axId val="2103720648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,14 +735,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120468296"/>
+        <c:crossAx val="2103717592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -769,7 +771,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1008,11 +1009,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="423147592"/>
-        <c:axId val="423136440"/>
+        <c:axId val="2103755912"/>
+        <c:axId val="2103758952"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="423147592"/>
+        <c:axId val="2103755912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,14 +1023,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="423136440"/>
+        <c:crossAx val="2103758952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="423136440"/>
+        <c:axId val="2103758952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1040,14 +1041,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="423147592"/>
+        <c:crossAx val="2103755912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1578,7 +1578,7 @@
         <v>31250</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C29" si="0">(B4-B3)/((A4-A3)/30.5)</f>
+        <f t="shared" ref="C4:C28" si="0">(B4-B3)/((A4-A3)/30.5)</f>
         <v>11678</v>
       </c>
       <c r="D4" s="2"/>
@@ -1604,6 +1604,12 @@
       <c r="E5" t="s">
         <v>2</v>
       </c>
+      <c r="K5">
+        <v>66529</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1">
@@ -1622,12 +1628,6 @@
       </c>
       <c r="E6" t="s">
         <v>2</v>
-      </c>
-      <c r="K6">
-        <v>66529</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:13">

</xml_diff>